<commit_message>
added the tiva seqgen_fast code
</commit_message>
<xml_diff>
--- a/homework3/timer_calc.xlsx
+++ b/homework3/timer_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arman\github\ecen5623-rtes\homework3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F51D6A-BBCA-4DEA-954B-A524A8CD2D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48EDDF-05FE-439D-921E-CA432EA1F9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2472" yWindow="3216" windowWidth="17280" windowHeight="9420" xr2:uid="{9EED9D9B-3FB5-4301-9EAC-2D9A738715AE}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{9EED9D9B-3FB5-4301-9EAC-2D9A738715AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +491,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -503,7 +503,7 @@
       </c>
       <c r="B8" s="2">
         <f>B6/B3</f>
-        <v>120000</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>